<commit_message>
add 1% norm error to clas6, clas6_d syst error is uncorrelated now
</commit_message>
<xml_diff>
--- a/data/JAM/10037.xlsx
+++ b/data/JAM/10037.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="old" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">raw!$A$1:$A$53</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">raw!$A$1:$A$53</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">raw!$A$1:$A$53</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">raw!$A$1:$A$53</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="44">
   <si>
     <t xml:space="preserve">E140X DIS Hydrogen reduced cros section - 4cm target (x=.1) &amp; 15cm (x=.35,.50)
 L. Tao, Ph.D. Thesis, The American University, 1994
@@ -392,12 +393,12 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="A2:A16 D25"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="84" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -857,30 +858,30 @@
   </sheetPr>
   <dimension ref="1:49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S8" activeCellId="1" sqref="A2:A16 S8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="11.8976744186047"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="17.3906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="9.26976744186046"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="9.1906976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="4" width="10.2558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.0604651162791"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="14.1953488372093"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="14.3581395348837"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="15.3395348837209"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="14.1953488372093"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="14.6837209302326"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="13.7023255813953"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="6" width="24.3674418604651"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="6" width="21.246511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="5" width="11.8976744186047"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="12.2232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="17.8837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="9.51627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="9.43255813953488"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="4" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.3860465116279"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="5" width="16.1627906976744"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="14.7674418604651"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="15.0976744186047"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="18.293023255814"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="14.0279069767442"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="6" width="25.0232558139535"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="6" width="21.8232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="5" width="12.2232558139535"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38390,21 +38391,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S16"/>
+  <dimension ref="1:16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A16"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="14" min="1" style="8" width="11.8976744186047"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="18.8697674418605"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="21.493023255814"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="26.1720930232558"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="10" width="18.8697674418605"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="10" width="22.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="8" width="11.8976744186047"/>
+    <col collapsed="false" hidden="false" max="13" min="1" style="8" width="12.2232558139535"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="9" width="19.3627906976744"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="26.9116279069767"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="10" width="19.3627906976744"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="10" width="23.2186046511628"/>
+    <col collapsed="false" hidden="false" max="1023" min="19" style="8" width="12.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="12.2232558139535"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38412,117 +38414,112 @@
         <v>32</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="J1" s="13" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="N1" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="O1" s="14" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="Q1" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="R1" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="15" t="s">
         <v>27</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C2" s="16" t="n">
+        <v>0.1</v>
+      </c>
       <c r="D2" s="16" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="16" t="n">
-        <v>0.5</v>
+        <v>3.3</v>
       </c>
       <c r="F2" s="16" t="n">
-        <v>3.3</v>
+        <v>0.636</v>
       </c>
       <c r="G2" s="16" t="n">
-        <v>0.636</v>
+        <v>28.261</v>
       </c>
       <c r="H2" s="16" t="n">
-        <v>28.261</v>
-      </c>
-      <c r="I2" s="16" t="n">
         <v>0.342</v>
       </c>
+      <c r="I2" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J2" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="8" t="n">
+      <c r="L2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N2" s="9" t="n">
+        <v>0.236740341418622</v>
+      </c>
       <c r="O2" s="9" t="n">
-        <v>0.236740341418622</v>
+        <v>0.953134510042605</v>
       </c>
       <c r="P2" s="9" t="n">
-        <v>0.953134510042605</v>
-      </c>
-      <c r="Q2" s="9" t="n">
         <v>0.692026780279976</v>
       </c>
-      <c r="R2" s="17" t="n">
+      <c r="Q2" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S2" s="17" t="n">
+      <c r="R2" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38531,58 +38528,55 @@
         <v>40</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C3" s="16" t="n">
+        <v>0.1</v>
+      </c>
       <c r="D3" s="16" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="16" t="n">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="16" t="n">
-        <v>4</v>
+        <v>1.336</v>
       </c>
       <c r="G3" s="16" t="n">
-        <v>1.336</v>
+        <v>17.598</v>
       </c>
       <c r="H3" s="16" t="n">
-        <v>17.598</v>
-      </c>
-      <c r="I3" s="16" t="n">
         <v>0.579</v>
       </c>
+      <c r="I3" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J3" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="8" t="n">
+      <c r="L3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N3" s="9" t="n">
+        <v>0.256509393794759</v>
+      </c>
       <c r="O3" s="9" t="n">
-        <v>0.256509393794759</v>
+        <v>0.745018679950187</v>
       </c>
       <c r="P3" s="9" t="n">
-        <v>0.745018679950187</v>
-      </c>
-      <c r="Q3" s="9" t="n">
         <v>0.707451224574512</v>
       </c>
-      <c r="R3" s="17" t="n">
+      <c r="Q3" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S3" s="17" t="n">
+      <c r="R3" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38591,58 +38585,55 @@
         <v>40</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C4" s="16" t="n">
+        <v>0.1</v>
+      </c>
       <c r="D4" s="16" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="16" t="n">
-        <v>0.5</v>
+        <v>4.95</v>
       </c>
       <c r="F4" s="16" t="n">
-        <v>4.95</v>
+        <v>2.286</v>
       </c>
       <c r="G4" s="16" t="n">
-        <v>2.286</v>
+        <v>12.067</v>
       </c>
       <c r="H4" s="16" t="n">
-        <v>12.067</v>
-      </c>
-      <c r="I4" s="16" t="n">
         <v>0.746</v>
       </c>
+      <c r="I4" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J4" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="8" t="n">
+      <c r="L4" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="M4" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N4" s="9" t="n">
+        <v>0.26517601599866</v>
+      </c>
       <c r="O4" s="9" t="n">
-        <v>0.26517601599866</v>
+        <v>0.625600698995194</v>
       </c>
       <c r="P4" s="9" t="n">
-        <v>0.625600698995194</v>
-      </c>
-      <c r="Q4" s="9" t="n">
         <v>0.740498034076016</v>
       </c>
-      <c r="R4" s="17" t="n">
+      <c r="Q4" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S4" s="17" t="n">
+      <c r="R4" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38651,58 +38642,55 @@
         <v>40</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C5" s="16" t="n">
+        <v>0.1</v>
+      </c>
       <c r="D5" s="16" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E5" s="16" t="n">
+        <v>6.45</v>
+      </c>
+      <c r="F5" s="16" t="n">
+        <v>1.121</v>
+      </c>
+      <c r="G5" s="16" t="n">
+        <v>21.432</v>
+      </c>
+      <c r="H5" s="16" t="n">
+        <v>0.322</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="16" t="n">
-        <v>6.45</v>
-      </c>
-      <c r="G5" s="16" t="n">
-        <v>1.121</v>
-      </c>
-      <c r="H5" s="16" t="n">
-        <v>21.432</v>
-      </c>
-      <c r="I5" s="16" t="n">
-        <v>0.322</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N5" s="9" t="n">
+        <v>0.275306736575512</v>
+      </c>
       <c r="O5" s="9" t="n">
-        <v>0.275306736575512</v>
+        <v>1.00618811881188</v>
       </c>
       <c r="P5" s="9" t="n">
-        <v>1.00618811881188</v>
-      </c>
-      <c r="Q5" s="9" t="n">
         <v>0.75990099009901</v>
       </c>
-      <c r="R5" s="17" t="n">
+      <c r="Q5" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S5" s="17" t="n">
+      <c r="R5" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38711,58 +38699,55 @@
         <v>40</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C6" s="16" t="n">
+        <v>0.1</v>
+      </c>
       <c r="D6" s="16" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E6" s="16" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="F6" s="16" t="n">
+        <v>1.571</v>
+      </c>
+      <c r="G6" s="16" t="n">
+        <v>17.47</v>
+      </c>
+      <c r="H6" s="16" t="n">
+        <v>0.419</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="16" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="G6" s="16" t="n">
-        <v>1.571</v>
-      </c>
-      <c r="H6" s="16" t="n">
-        <v>17.47</v>
-      </c>
-      <c r="I6" s="16" t="n">
-        <v>0.419</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" s="16" t="s">
+      <c r="M6" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N6" s="9" t="n">
+        <v>0.283042980790732</v>
+      </c>
       <c r="O6" s="9" t="n">
-        <v>0.283042980790732</v>
+        <v>1.48601811736904</v>
       </c>
       <c r="P6" s="9" t="n">
-        <v>1.48601811736904</v>
-      </c>
-      <c r="Q6" s="9" t="n">
         <v>0.70106341079165</v>
       </c>
-      <c r="R6" s="17" t="n">
+      <c r="Q6" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S6" s="17" t="n">
+      <c r="R6" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38771,58 +38756,55 @@
         <v>40</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C7" s="16" t="n">
+        <v>0.1</v>
+      </c>
       <c r="D7" s="16" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E7" s="16" t="n">
+        <v>7.99</v>
+      </c>
+      <c r="F7" s="16" t="n">
+        <v>2.661</v>
+      </c>
+      <c r="G7" s="16" t="n">
+        <v>12.45</v>
+      </c>
+      <c r="H7" s="16" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="16" t="n">
-        <v>7.99</v>
-      </c>
-      <c r="G7" s="16" t="n">
-        <v>2.661</v>
-      </c>
-      <c r="H7" s="16" t="n">
-        <v>12.45</v>
-      </c>
-      <c r="I7" s="16" t="n">
-        <v>0.588</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="16" t="s">
+      <c r="M7" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N7" s="9" t="n">
+        <v>0.303598342827263</v>
+      </c>
       <c r="O7" s="9" t="n">
-        <v>0.303598342827263</v>
+        <v>0.766755555555555</v>
       </c>
       <c r="P7" s="9" t="n">
-        <v>0.766755555555555</v>
-      </c>
-      <c r="Q7" s="9" t="n">
         <v>0.718933333333333</v>
       </c>
-      <c r="R7" s="17" t="n">
+      <c r="Q7" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S7" s="17" t="n">
+      <c r="R7" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38831,58 +38813,55 @@
         <v>40</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C8" s="16" t="n">
+        <v>0.35</v>
+      </c>
       <c r="D8" s="16" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E8" s="16" t="n">
-        <v>3</v>
+        <v>5.6</v>
       </c>
       <c r="F8" s="16" t="n">
-        <v>5.6</v>
+        <v>1.032</v>
       </c>
       <c r="G8" s="16" t="n">
-        <v>1.032</v>
+        <v>42.223</v>
       </c>
       <c r="H8" s="16" t="n">
-        <v>42.223</v>
-      </c>
-      <c r="I8" s="16" t="n">
         <v>0.297</v>
       </c>
+      <c r="I8" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J8" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="8" t="n">
+      <c r="L8" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="M8" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N8" s="9" t="n">
+        <v>0.246273142430797</v>
+      </c>
       <c r="O8" s="9" t="n">
-        <v>0.246273142430797</v>
+        <v>1.1956241956242</v>
       </c>
       <c r="P8" s="9" t="n">
-        <v>1.1956241956242</v>
-      </c>
-      <c r="Q8" s="9" t="n">
         <v>0.705276705276705</v>
       </c>
-      <c r="R8" s="17" t="n">
+      <c r="Q8" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S8" s="17" t="n">
+      <c r="R8" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38891,58 +38870,55 @@
         <v>40</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C9" s="16" t="n">
+        <v>0.35</v>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>3</v>
+        <v>6.45</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>6.45</v>
+        <v>1.882</v>
       </c>
       <c r="G9" s="16" t="n">
-        <v>1.882</v>
+        <v>28.783</v>
       </c>
       <c r="H9" s="16" t="n">
-        <v>28.783</v>
-      </c>
-      <c r="I9" s="16" t="n">
         <v>0.488</v>
       </c>
+      <c r="I9" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J9" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="8" t="n">
+      <c r="L9" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N9" s="9" t="n">
+        <v>0.249068667492659</v>
+      </c>
       <c r="O9" s="9" t="n">
-        <v>0.249068667492659</v>
+        <v>0.867329047340736</v>
       </c>
       <c r="P9" s="9" t="n">
-        <v>0.867329047340736</v>
-      </c>
-      <c r="Q9" s="9" t="n">
         <v>0.715371127995324</v>
       </c>
-      <c r="R9" s="17" t="n">
+      <c r="Q9" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S9" s="17" t="n">
+      <c r="R9" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -38951,58 +38927,55 @@
         <v>40</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C10" s="16" t="n">
+        <v>0.35</v>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E10" s="16" t="n">
-        <v>3</v>
+        <v>7.99</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>7.99</v>
+        <v>3.422</v>
       </c>
       <c r="G10" s="16" t="n">
-        <v>3.422</v>
+        <v>19.066</v>
       </c>
       <c r="H10" s="16" t="n">
-        <v>19.066</v>
-      </c>
-      <c r="I10" s="16" t="n">
         <v>0.69</v>
       </c>
+      <c r="I10" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J10" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="8" t="n">
+      <c r="L10" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N10" s="16" t="s">
+      <c r="M10" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N10" s="9" t="n">
+        <v>0.261079593764419</v>
+      </c>
       <c r="O10" s="9" t="n">
-        <v>0.261079593764419</v>
+        <v>0.656472752356864</v>
       </c>
       <c r="P10" s="9" t="n">
-        <v>0.656472752356864</v>
-      </c>
-      <c r="Q10" s="9" t="n">
         <v>0.729937916762474</v>
       </c>
-      <c r="R10" s="17" t="n">
+      <c r="Q10" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S10" s="17" t="n">
+      <c r="R10" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -39011,58 +38984,55 @@
         <v>40</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C11" s="16" t="n">
+        <v>0.35</v>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="E11" s="16" t="n">
-        <v>3</v>
+        <v>9.75</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>9.75</v>
+        <v>5.182</v>
       </c>
       <c r="G11" s="16" t="n">
-        <v>5.182</v>
+        <v>13.996</v>
       </c>
       <c r="H11" s="16" t="n">
-        <v>13.996</v>
-      </c>
-      <c r="I11" s="16" t="n">
         <v>0.807</v>
       </c>
+      <c r="I11" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J11" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="8" t="n">
+      <c r="L11" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N11" s="9" t="n">
+        <v>0.266517846829264</v>
+      </c>
       <c r="O11" s="9" t="n">
-        <v>0.266517846829264</v>
+        <v>0.69971671388102</v>
       </c>
       <c r="P11" s="9" t="n">
-        <v>0.69971671388102</v>
-      </c>
-      <c r="Q11" s="9" t="n">
         <v>0.751841359773371</v>
       </c>
-      <c r="R11" s="17" t="n">
+      <c r="Q11" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S11" s="17" t="n">
+      <c r="R11" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -39071,58 +39041,55 @@
         <v>40</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C12" s="16" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E12" s="16" t="n">
-        <v>3.6</v>
+        <v>4.95</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>4.95</v>
+        <v>1.113</v>
       </c>
       <c r="G12" s="16" t="n">
-        <v>1.113</v>
+        <v>47.675</v>
       </c>
       <c r="H12" s="16" t="n">
-        <v>47.675</v>
-      </c>
-      <c r="I12" s="16" t="n">
         <v>0.335</v>
       </c>
+      <c r="I12" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J12" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M12" s="8" t="n">
+      <c r="L12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N12" s="16" t="s">
+      <c r="M12" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N12" s="9" t="n">
+        <v>0.154459868935607</v>
+      </c>
       <c r="O12" s="9" t="n">
-        <v>0.154459868935607</v>
+        <v>1.26644118752349</v>
       </c>
       <c r="P12" s="9" t="n">
-        <v>1.26644118752349</v>
-      </c>
-      <c r="Q12" s="9" t="n">
         <v>0.81072278592008</v>
       </c>
-      <c r="R12" s="17" t="n">
+      <c r="Q12" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S12" s="17" t="n">
+      <c r="R12" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -39131,58 +39098,55 @@
         <v>40</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C13" s="16" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D13" s="16" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E13" s="16" t="n">
-        <v>3.6</v>
+        <v>5.6</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>5.6</v>
+        <v>1.763</v>
       </c>
       <c r="G13" s="16" t="n">
-        <v>1.763</v>
+        <v>35.145</v>
       </c>
       <c r="H13" s="16" t="n">
-        <v>35.145</v>
-      </c>
-      <c r="I13" s="16" t="n">
         <v>0.495</v>
       </c>
+      <c r="I13" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J13" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M13" s="8" t="n">
+      <c r="L13" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N13" s="16" t="s">
+      <c r="M13" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N13" s="9" t="n">
+        <v>0.157395394316431</v>
+      </c>
       <c r="O13" s="9" t="n">
-        <v>0.157395394316431</v>
+        <v>0.783333333333333</v>
       </c>
       <c r="P13" s="9" t="n">
-        <v>0.783333333333333</v>
-      </c>
-      <c r="Q13" s="9" t="n">
         <v>0.757333333333334</v>
       </c>
-      <c r="R13" s="17" t="n">
+      <c r="Q13" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S13" s="17" t="n">
+      <c r="R13" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -39191,58 +39155,55 @@
         <v>40</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C14" s="16" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D14" s="16" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E14" s="16" t="n">
-        <v>3.6</v>
+        <v>6.45</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>6.45</v>
+        <v>2.613</v>
       </c>
       <c r="G14" s="16" t="n">
-        <v>2.613</v>
+        <v>26.721</v>
       </c>
       <c r="H14" s="16" t="n">
-        <v>26.721</v>
-      </c>
-      <c r="I14" s="16" t="n">
         <v>0.635</v>
       </c>
+      <c r="I14" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J14" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="8" t="n">
+      <c r="L14" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N14" s="16" t="s">
+      <c r="M14" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N14" s="9" t="n">
+        <v>0.163790377422423</v>
+      </c>
       <c r="O14" s="9" t="n">
-        <v>0.163790377422423</v>
+        <v>0.53019410496046</v>
       </c>
       <c r="P14" s="9" t="n">
-        <v>0.53019410496046</v>
-      </c>
-      <c r="Q14" s="9" t="n">
         <v>0.824586628324946</v>
       </c>
-      <c r="R14" s="17" t="n">
+      <c r="Q14" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S14" s="17" t="n">
+      <c r="R14" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -39251,58 +39212,55 @@
         <v>40</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C15" s="16" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D15" s="16" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E15" s="16" t="n">
-        <v>3.6</v>
+        <v>6.9</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>6.9</v>
+        <v>3.063</v>
       </c>
       <c r="G15" s="16" t="n">
-        <v>3.063</v>
+        <v>23.817</v>
       </c>
       <c r="H15" s="16" t="n">
-        <v>23.817</v>
-      </c>
-      <c r="I15" s="16" t="n">
         <v>0.688</v>
       </c>
+      <c r="I15" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J15" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M15" s="8" t="n">
+      <c r="L15" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N15" s="16" t="s">
+      <c r="M15" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N15" s="9" t="n">
+        <v>0.159661450626291</v>
+      </c>
       <c r="O15" s="9" t="n">
-        <v>0.159661450626291</v>
+        <v>1.03306497987349</v>
       </c>
       <c r="P15" s="9" t="n">
-        <v>1.03306497987349</v>
-      </c>
-      <c r="Q15" s="9" t="n">
         <v>0.794134560092007</v>
       </c>
-      <c r="R15" s="17" t="n">
+      <c r="Q15" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S15" s="17" t="n">
+      <c r="R15" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -39311,58 +39269,55 @@
         <v>40</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="C16" s="16" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D16" s="16" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="E16" s="16" t="n">
-        <v>3.6</v>
+        <v>9.75</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>9.75</v>
+        <v>5.913</v>
       </c>
       <c r="G16" s="16" t="n">
-        <v>5.913</v>
+        <v>14.355</v>
       </c>
       <c r="H16" s="16" t="n">
-        <v>14.355</v>
-      </c>
-      <c r="I16" s="16" t="n">
         <v>0.861</v>
       </c>
+      <c r="I16" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="J16" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M16" s="8" t="n">
+      <c r="L16" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N16" s="16" t="s">
+      <c r="M16" s="16" t="s">
         <v>5</v>
       </c>
+      <c r="N16" s="9" t="n">
+        <v>0.1685746703143</v>
+      </c>
       <c r="O16" s="9" t="n">
-        <v>0.1685746703143</v>
+        <v>0.607733333333333</v>
       </c>
       <c r="P16" s="9" t="n">
-        <v>0.607733333333333</v>
-      </c>
-      <c r="Q16" s="9" t="n">
         <v>0.8256</v>
       </c>
-      <c r="R16" s="17" t="n">
+      <c r="Q16" s="17" t="n">
         <f aca="false">SQRT(3)</f>
         <v>1.73205080756888</v>
       </c>
-      <c r="S16" s="17" t="n">
+      <c r="R16" s="17" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>